<commit_message>
File  list name changed
</commit_message>
<xml_diff>
--- a/File9.xlsx
+++ b/File9.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="480" yWindow="345" windowWidth="19875" windowHeight="7725"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Bug report" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -480,7 +480,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>